<commit_message>
Add the report and presentation files
</commit_message>
<xml_diff>
--- a/MySEProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
+++ b/MySEProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\MySEProject\Dataset Reports\Dataset-GurunagSai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22130B3A-4858-471D-9529-68FBDE653F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D081C40-1C35-46CF-AA4C-DD08FA9B18D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="148">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -147,10 +147,6 @@
 macro corelation(36-1.8%) micro corelation(81-40%)</t>
   </si>
   <si>
-    <t>Valid output
-macro corelation(57-17%) micro corelation(89-64%)</t>
-  </si>
-  <si>
     <t>output-21</t>
   </si>
   <si>
@@ -485,15 +481,76 @@
     <t>valid output macro corelation(46-4%) micro corelation(87-47%)</t>
   </si>
   <si>
-    <t>Better output micro(92-75) and macro(68-45)</t>
+    <t>Experiments  with potential radiius 1</t>
+  </si>
+  <si>
+    <t>output-67</t>
+  </si>
+  <si>
+    <t>output-68</t>
+  </si>
+  <si>
+    <t>output-69</t>
+  </si>
+  <si>
+    <t>output-70</t>
+  </si>
+  <si>
+    <t>output-71</t>
+  </si>
+  <si>
+    <t>output-72</t>
+  </si>
+  <si>
+    <t>output-73</t>
+  </si>
+  <si>
+    <t>output-74</t>
+  </si>
+  <si>
+    <t>variance is very high between the max and min value</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">BEST OUTPUT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>macro corelation(57-17%) micro corelation(89-64%)</t>
+    </r>
+  </si>
+  <si>
+    <t>valid output micro(92-75) and macro(68-45)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -598,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -618,15 +675,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -645,6 +693,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -925,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O84" sqref="O84"/>
+    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,24 +1004,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>61</v>
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
@@ -977,17 +1035,17 @@
         <v>2</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>130</v>
+        <v>98</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1158,7 +1216,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>19</v>
@@ -1187,7 +1245,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>19</v>
@@ -1216,7 +1274,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>19</v>
@@ -1239,16 +1297,16 @@
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1268,16 +1326,16 @@
         <v>20</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1297,16 +1355,16 @@
         <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1326,16 +1384,16 @@
         <v>100</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1355,16 +1413,16 @@
         <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1384,16 +1442,16 @@
         <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1413,16 +1471,16 @@
         <v>100</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1448,10 +1506,10 @@
         <v>5</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1477,10 +1535,10 @@
         <v>5</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1506,15 +1564,15 @@
         <v>5</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>131</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1630,7 +1688,7 @@
         <v>22</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1659,7 +1717,7 @@
         <v>23</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1679,30 +1737,30 @@
         <v>100</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -1730,7 +1788,7 @@
         <v>13</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1759,7 +1817,7 @@
         <v>24</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1849,9 +1907,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>134</v>
+    <row r="35" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1880,7 +1938,7 @@
         <v>14</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1908,8 +1966,8 @@
       <c r="H37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>37</v>
+      <c r="I37" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2022,10 +2080,10 @@
         <v>5</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2051,10 +2109,10 @@
         <v>5</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2080,10 +2138,10 @@
         <v>5</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2109,10 +2167,10 @@
         <v>5</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2138,10 +2196,10 @@
         <v>5</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2167,10 +2225,10 @@
         <v>5</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2196,15 +2254,15 @@
         <v>5</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>133</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2230,10 +2288,10 @@
         <v>5</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2259,10 +2317,10 @@
         <v>5</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2288,10 +2346,10 @@
         <v>5</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2317,10 +2375,10 @@
         <v>5</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2346,10 +2404,10 @@
         <v>5</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2375,10 +2433,10 @@
         <v>5</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2404,10 +2462,10 @@
         <v>5</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2433,10 +2491,10 @@
         <v>5</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2462,10 +2520,10 @@
         <v>5</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2491,10 +2549,10 @@
         <v>5</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2520,10 +2578,10 @@
         <v>5</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2549,10 +2607,10 @@
         <v>5</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2578,10 +2636,10 @@
         <v>5</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2607,10 +2665,10 @@
         <v>5</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2636,10 +2694,10 @@
         <v>5</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2665,10 +2723,10 @@
         <v>5</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2694,10 +2752,10 @@
         <v>5</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2723,10 +2781,10 @@
         <v>5</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2752,10 +2810,10 @@
         <v>5</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2781,10 +2839,10 @@
         <v>5</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2810,10 +2868,10 @@
         <v>5</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2839,10 +2897,10 @@
         <v>5</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2868,10 +2926,10 @@
         <v>5</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2897,10 +2955,10 @@
         <v>5</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2926,23 +2984,261 @@
         <v>5</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="18">
+        <v>67</v>
+      </c>
+      <c r="B75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C75" s="18">
+        <v>1</v>
+      </c>
+      <c r="D75" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="E75" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="18">
+        <v>68</v>
+      </c>
+      <c r="B76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C76" s="18">
+        <v>1</v>
+      </c>
+      <c r="D76" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="E76" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="18">
+        <v>69</v>
+      </c>
+      <c r="B77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C77" s="18">
+        <v>1</v>
+      </c>
+      <c r="D77" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="E77" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H77" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="18">
+        <v>70</v>
+      </c>
+      <c r="B78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C78" s="18">
+        <v>1</v>
+      </c>
+      <c r="D78" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E78" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H78" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="18">
+        <v>71</v>
+      </c>
+      <c r="B79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C79" s="18">
+        <v>1</v>
+      </c>
+      <c r="D79" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="E79" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H79" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="18">
+        <v>72</v>
+      </c>
+      <c r="B80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C80" s="18">
+        <v>1</v>
+      </c>
+      <c r="D80" s="18">
+        <v>0.7</v>
+      </c>
+      <c r="E80" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H80" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="18">
+        <v>73</v>
+      </c>
+      <c r="B81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C81" s="18">
+        <v>1</v>
+      </c>
+      <c r="D81" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="E81" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H81" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="18">
+        <v>74</v>
+      </c>
+      <c r="B82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C82" s="18">
+        <v>1</v>
+      </c>
+      <c r="D82" s="18">
+        <v>0.9</v>
+      </c>
+      <c r="E82" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H82" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A22:XFD22"/>
+    <mergeCell ref="A29:XFD29"/>
+    <mergeCell ref="A35:XFD35"/>
+    <mergeCell ref="A48:XFD48"/>
+    <mergeCell ref="A74:XFD74"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="A3:XFD3"/>
-    <mergeCell ref="A22:XFD22"/>
-    <mergeCell ref="A29:XFD29"/>
-    <mergeCell ref="A35:XFD35"/>
-    <mergeCell ref="A48:XFD48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>